<commit_message>
testing N bulk instead of N throughfall
</commit_message>
<xml_diff>
--- a/data/ICP_Level_II_sites_N_data_2021.xlsx
+++ b/data/ICP_Level_II_sites_N_data_2021.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Tresch IAP\Desktop\IAP\1_Projects\11_UNECE\N_leaching_CLempN\N_leaching_analysis_CLempN\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A12B41D-35D1-4C86-8919-0E64E7D7AC76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299A0E4-F1F8-4616-9C11-163CBBDEE17A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0287CEAC-16CA-4849-9678-E41A93D51B23}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICP Level II N data" sheetId="1" r:id="rId1"/>
@@ -165,9 +164,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>N_troughfall</t>
-  </si>
-  <si>
     <t>N_precipitation</t>
   </si>
   <si>
@@ -316,6 +312,9 @@
   </si>
   <si>
     <t>CH - Sabine Braun and Simon Tresch</t>
+  </si>
+  <si>
+    <t>N_throughfall</t>
   </si>
 </sst>
 </file>
@@ -678,11 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="1">
-      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1047,7 +1043,7 @@
         <v>33</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1080,10 +1076,10 @@
         <v>30</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1116,7 +1112,7 @@
         <v>25</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1149,18 +1145,18 @@
         <v>23</v>
       </c>
       <c r="J17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
       <c r="D18">
         <v>550.98800000000006</v>
@@ -1180,13 +1176,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
       <c r="D19">
         <v>978.95442447999994</v>
@@ -1204,21 +1200,21 @@
         <v>22.235628105039041</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <v>806.226</v>
@@ -1236,18 +1232,18 @@
         <v>19.578713968957874</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>595.55799999999999</v>
@@ -1265,18 +1261,18 @@
         <v>24.750869061413677</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22">
         <v>719.49</v>
@@ -1291,21 +1287,21 @@
         <v>0.15951463899387702</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23">
         <v>699.62</v>
@@ -1323,18 +1319,18 @@
         <v>25.102339181286542</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24">
         <v>623.08800000000008</v>
@@ -1352,18 +1348,18 @@
         <v>25.774253731343286</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25">
         <v>900.53513793160073</v>
@@ -1381,18 +1377,18 @@
         <v>23.438651766795143</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26">
         <v>1732.3383999999999</v>
@@ -1410,15 +1406,15 @@
         <v>19.333333333333336</v>
       </c>
       <c r="J26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
@@ -1439,18 +1435,18 @@
         <v>26.447931526390871</v>
       </c>
       <c r="J27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28">
         <v>659.34555632000001</v>
@@ -1468,18 +1464,18 @@
         <v>23.52</v>
       </c>
       <c r="J28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29">
         <v>651.52472513999999</v>
@@ -1497,18 +1493,18 @@
         <v>27.352368591823492</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30">
         <v>1185.3579999999999</v>
@@ -1526,18 +1522,18 @@
         <v>19.936373276776248</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31">
         <v>1091.7305349600001</v>
@@ -1555,18 +1551,18 @@
         <v>21.368560990373656</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32">
         <v>751.73521962011046</v>
@@ -1584,12 +1580,12 @@
         <v>22.740963855421686</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J33" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1607,7 +1603,6 @@
       <selection activeCell="F3" sqref="F3"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D17:D21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4645,12 +4640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFB1B43-A2CF-41A2-B653-1C573349BF1F}">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4663,7 +4654,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
@@ -4678,25 +4669,25 @@
         <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
         <v>39</v>
       </c>
       <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>48</v>
-      </c>
-      <c r="L1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -4716,7 +4707,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2">
         <v>2002</v>
@@ -4754,7 +4745,7 @@
         <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3">
         <v>2003</v>
@@ -4792,7 +4783,7 @@
         <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4">
         <v>2004</v>
@@ -4830,7 +4821,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5">
         <v>2005</v>
@@ -4868,7 +4859,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6">
         <v>2006</v>
@@ -4906,7 +4897,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7">
         <v>2007</v>
@@ -4944,7 +4935,7 @@
         <v>31</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8">
         <v>2008</v>
@@ -4982,7 +4973,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9">
         <v>2009</v>
@@ -5020,7 +5011,7 @@
         <v>31</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10">
         <v>2010</v>
@@ -5058,7 +5049,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11">
         <v>2011</v>
@@ -5096,7 +5087,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12">
         <v>2012</v>
@@ -5134,7 +5125,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13">
         <v>2013</v>
@@ -5172,7 +5163,7 @@
         <v>31</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14">
         <v>2014</v>
@@ -5210,7 +5201,7 @@
         <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15">
         <v>2015</v>
@@ -5248,7 +5239,7 @@
         <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16">
         <v>2016</v>
@@ -5286,7 +5277,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17">
         <v>2017</v>
@@ -5324,7 +5315,7 @@
         <v>31</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18">
         <v>2018</v>
@@ -5362,7 +5353,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G19">
         <v>2019</v>
@@ -5400,7 +5391,7 @@
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20">
         <v>1997</v>
@@ -5438,7 +5429,7 @@
         <v>33</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21">
         <v>1998</v>
@@ -5476,7 +5467,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G22">
         <v>1999</v>
@@ -5514,7 +5505,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G23">
         <v>2000</v>
@@ -5552,7 +5543,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24">
         <v>2001</v>
@@ -5590,7 +5581,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25">
         <v>2002</v>
@@ -5628,7 +5619,7 @@
         <v>33</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G26">
         <v>2003</v>
@@ -5666,7 +5657,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27">
         <v>2004</v>
@@ -5704,7 +5695,7 @@
         <v>33</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G28">
         <v>2005</v>
@@ -5742,7 +5733,7 @@
         <v>33</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G29">
         <v>2006</v>
@@ -5780,7 +5771,7 @@
         <v>33</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G30">
         <v>2007</v>
@@ -5818,7 +5809,7 @@
         <v>33</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G31">
         <v>2008</v>
@@ -5856,7 +5847,7 @@
         <v>33</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G32">
         <v>2009</v>
@@ -5894,7 +5885,7 @@
         <v>33</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G33">
         <v>2010</v>
@@ -5932,7 +5923,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G34">
         <v>2011</v>
@@ -5970,7 +5961,7 @@
         <v>33</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G35">
         <v>2012</v>
@@ -6008,7 +5999,7 @@
         <v>33</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G36">
         <v>2013</v>
@@ -6046,7 +6037,7 @@
         <v>33</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G37">
         <v>2014</v>
@@ -6084,7 +6075,7 @@
         <v>33</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G38">
         <v>2015</v>
@@ -6122,7 +6113,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G39">
         <v>2016</v>
@@ -6160,7 +6151,7 @@
         <v>33</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G40">
         <v>2017</v>
@@ -6198,7 +6189,7 @@
         <v>33</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G41">
         <v>2018</v>
@@ -6236,7 +6227,7 @@
         <v>33</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G42">
         <v>2019</v>
@@ -6274,7 +6265,7 @@
         <v>15</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G43">
         <v>1997</v>
@@ -6312,7 +6303,7 @@
         <v>15</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G44">
         <v>1998</v>
@@ -6350,7 +6341,7 @@
         <v>15</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G45">
         <v>1999</v>
@@ -6388,7 +6379,7 @@
         <v>15</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G46">
         <v>2000</v>
@@ -6426,7 +6417,7 @@
         <v>15</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G47">
         <v>2001</v>
@@ -6464,7 +6455,7 @@
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G48">
         <v>2002</v>
@@ -6502,7 +6493,7 @@
         <v>15</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G49">
         <v>2003</v>
@@ -6540,7 +6531,7 @@
         <v>15</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G50">
         <v>2004</v>
@@ -6578,7 +6569,7 @@
         <v>15</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G51">
         <v>2005</v>
@@ -6616,7 +6607,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G52">
         <v>2006</v>
@@ -6654,7 +6645,7 @@
         <v>15</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G53">
         <v>2007</v>
@@ -6692,7 +6683,7 @@
         <v>15</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G54">
         <v>2008</v>
@@ -6730,7 +6721,7 @@
         <v>15</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G55">
         <v>2009</v>
@@ -6768,7 +6759,7 @@
         <v>15</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G56">
         <v>2010</v>
@@ -6806,7 +6797,7 @@
         <v>15</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G57">
         <v>2011</v>
@@ -6844,7 +6835,7 @@
         <v>15</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G58">
         <v>2012</v>
@@ -6882,7 +6873,7 @@
         <v>15</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G59">
         <v>2013</v>
@@ -6920,7 +6911,7 @@
         <v>15</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G60">
         <v>2014</v>
@@ -6958,7 +6949,7 @@
         <v>15</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G61">
         <v>2015</v>
@@ -6996,7 +6987,7 @@
         <v>15</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G62">
         <v>2016</v>
@@ -7034,7 +7025,7 @@
         <v>15</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G63">
         <v>2017</v>
@@ -7072,7 +7063,7 @@
         <v>15</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G64">
         <v>2018</v>
@@ -7110,7 +7101,7 @@
         <v>15</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G65">
         <v>2019</v>
@@ -7148,7 +7139,7 @@
         <v>32</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G66">
         <v>1994</v>
@@ -7186,7 +7177,7 @@
         <v>32</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G67">
         <v>1995</v>
@@ -7224,7 +7215,7 @@
         <v>32</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G68">
         <v>1996</v>
@@ -7262,7 +7253,7 @@
         <v>32</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G69">
         <v>1997</v>
@@ -7300,7 +7291,7 @@
         <v>32</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G70">
         <v>1998</v>
@@ -7338,7 +7329,7 @@
         <v>32</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G71">
         <v>1999</v>
@@ -7376,7 +7367,7 @@
         <v>32</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G72">
         <v>2000</v>
@@ -7414,7 +7405,7 @@
         <v>32</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G73">
         <v>2001</v>
@@ -7452,7 +7443,7 @@
         <v>32</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G74">
         <v>2002</v>
@@ -7490,7 +7481,7 @@
         <v>32</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G75">
         <v>2003</v>
@@ -7528,7 +7519,7 @@
         <v>32</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G76">
         <v>2004</v>
@@ -7566,7 +7557,7 @@
         <v>32</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G77">
         <v>2005</v>
@@ -7604,7 +7595,7 @@
         <v>32</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G78">
         <v>2006</v>
@@ -7642,7 +7633,7 @@
         <v>32</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G79">
         <v>2007</v>
@@ -7680,7 +7671,7 @@
         <v>32</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G80">
         <v>2008</v>
@@ -7718,7 +7709,7 @@
         <v>32</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G81">
         <v>2009</v>
@@ -7756,7 +7747,7 @@
         <v>32</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G82">
         <v>2010</v>
@@ -7794,7 +7785,7 @@
         <v>32</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G83">
         <v>2011</v>
@@ -7832,7 +7823,7 @@
         <v>32</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G84">
         <v>2012</v>
@@ -7870,7 +7861,7 @@
         <v>32</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G85">
         <v>2013</v>
@@ -7908,7 +7899,7 @@
         <v>32</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G86">
         <v>2014</v>
@@ -7946,7 +7937,7 @@
         <v>32</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G87">
         <v>2015</v>
@@ -7984,7 +7975,7 @@
         <v>32</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G88">
         <v>2016</v>
@@ -8022,7 +8013,7 @@
         <v>32</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G89">
         <v>2017</v>
@@ -8060,7 +8051,7 @@
         <v>32</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G90">
         <v>2018</v>
@@ -8098,7 +8089,7 @@
         <v>32</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G91">
         <v>2019</v>
@@ -8136,7 +8127,7 @@
         <v>31</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G92">
         <v>1996</v>
@@ -8174,7 +8165,7 @@
         <v>31</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G93">
         <v>1997</v>
@@ -8212,7 +8203,7 @@
         <v>31</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G94">
         <v>1998</v>
@@ -8250,7 +8241,7 @@
         <v>31</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G95">
         <v>1999</v>
@@ -8288,7 +8279,7 @@
         <v>31</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G96">
         <v>2000</v>
@@ -8326,7 +8317,7 @@
         <v>31</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G97">
         <v>2001</v>
@@ -8364,7 +8355,7 @@
         <v>31</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G98">
         <v>2002</v>
@@ -8402,7 +8393,7 @@
         <v>31</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G99">
         <v>2003</v>
@@ -8440,7 +8431,7 @@
         <v>31</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G100">
         <v>2004</v>
@@ -8478,7 +8469,7 @@
         <v>31</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G101">
         <v>2005</v>
@@ -8516,7 +8507,7 @@
         <v>31</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G102">
         <v>2006</v>
@@ -8554,7 +8545,7 @@
         <v>31</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G103">
         <v>2007</v>
@@ -8592,7 +8583,7 @@
         <v>31</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G104">
         <v>2008</v>
@@ -8630,7 +8621,7 @@
         <v>31</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G105">
         <v>2009</v>
@@ -8668,7 +8659,7 @@
         <v>31</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G106">
         <v>2010</v>
@@ -8706,7 +8697,7 @@
         <v>31</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G107">
         <v>2011</v>
@@ -8744,7 +8735,7 @@
         <v>31</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G108">
         <v>2012</v>
@@ -8782,7 +8773,7 @@
         <v>31</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G109">
         <v>2013</v>
@@ -8820,7 +8811,7 @@
         <v>31</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G110">
         <v>2014</v>
@@ -8858,7 +8849,7 @@
         <v>31</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G111">
         <v>2015</v>
@@ -8896,7 +8887,7 @@
         <v>31</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G112">
         <v>2016</v>
@@ -8934,7 +8925,7 @@
         <v>31</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G113">
         <v>2017</v>
@@ -8972,7 +8963,7 @@
         <v>31</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G114">
         <v>2018</v>
@@ -9010,7 +9001,7 @@
         <v>31</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G115">
         <v>2019</v>
@@ -9045,7 +9036,7 @@
         <v>14</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H116">
         <v>7.8575224718590695</v>
@@ -9077,7 +9068,7 @@
         <v>14</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H117">
         <v>16.248109738029164</v>
@@ -9109,7 +9100,7 @@
         <v>14</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H118">
         <v>12.91438003683859</v>
@@ -9141,7 +9132,7 @@
         <v>15</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H119">
         <v>15.0489904293331</v>
@@ -9173,7 +9164,7 @@
         <v>15</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H120">
         <v>11.720490270820212</v>
@@ -9205,7 +9196,7 @@
         <v>15</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H121">
         <v>2.9276904219806621</v>
@@ -9237,7 +9228,7 @@
         <v>16</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H122">
         <v>8.9030978476249469</v>
@@ -9269,7 +9260,7 @@
         <v>16</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H123">
         <v>3.3152522724761826</v>
@@ -9301,7 +9292,7 @@
         <v>16</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H124">
         <v>9.5213671855321333</v>
@@ -9321,19 +9312,19 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B125" t="s">
+        <v>50</v>
+      </c>
+      <c r="D125" t="s">
         <v>51</v>
       </c>
-      <c r="D125" t="s">
+      <c r="E125" t="s">
         <v>52</v>
       </c>
-      <c r="E125" t="s">
-        <v>53</v>
-      </c>
       <c r="F125" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H125" s="5">
         <v>11.564444802078857</v>
@@ -9353,19 +9344,19 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B126" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D126" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E126" t="s">
+        <v>84</v>
+      </c>
+      <c r="F126" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="F126" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="H126" s="5">
         <v>5.9876524580645158</v>
@@ -9385,19 +9376,19 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D127" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E127" t="s">
+        <v>84</v>
+      </c>
+      <c r="F127" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="H127" s="5">
         <v>10.984452582795701</v>
@@ -9417,19 +9408,19 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B128" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D128" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E128" t="s">
+        <v>84</v>
+      </c>
+      <c r="F128" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="F128" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="H128" s="5">
         <v>13.241655592114695</v>
@@ -9449,19 +9440,19 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B129" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D129" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E129" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H129" s="5">
         <v>11.569038514695343</v>
@@ -9479,19 +9470,19 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B130" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D130" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E130" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H130" s="5">
         <v>6.3634249677419374</v>
@@ -9511,19 +9502,19 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B131" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D131" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E131" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H131" s="5">
         <v>7.5418663770609324</v>
@@ -9543,19 +9534,19 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B132" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D132" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E132" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H132" s="5">
         <v>4.3580828238166855</v>
@@ -9575,19 +9566,19 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B133" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D133" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E133" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H133" s="5">
         <v>10.807116559856631</v>
@@ -9607,19 +9598,19 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B134" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D134" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E134" t="s">
         <v>15</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H134" s="5">
         <v>9.735613550042526</v>
@@ -9639,19 +9630,19 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B135" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D135" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E135" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H135" s="5">
         <v>20.540624754121868</v>
@@ -9671,19 +9662,19 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B136" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D136" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E136" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H136" s="5">
         <v>12.675100006227321</v>
@@ -9703,19 +9694,19 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B137" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D137" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E137" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H137" s="5">
         <v>41.726440677419355</v>
@@ -9735,19 +9726,19 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B138" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D138" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E138" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H138" s="5">
         <v>16.313251271684589</v>
@@ -9767,19 +9758,19 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B139" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D139" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E139" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H139" s="5">
         <v>11.54539542866083</v>

</xml_diff>

<commit_message>
data corrections Arne (BE)
</commit_message>
<xml_diff>
--- a/data/ICP_Level_II_sites_N_data_2021.xlsx
+++ b/data/ICP_Level_II_sites_N_data_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Tresch IAP\Desktop\IAP\1_Projects\11_UNECE\N_leaching_CLempN\N_leaching_analysis_CLempN\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2603F79-EFD6-4B5D-A4ED-1A17845A9F24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68B48F6-5362-4669-94E0-A01BC6ED77BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47025" yWindow="1260" windowWidth="13830" windowHeight="7170" firstSheet="1" activeTab="2" xr2:uid="{4B878E5B-3B0D-4C3A-956A-F5942ADBA4FC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="2" xr2:uid="{4B878E5B-3B0D-4C3A-956A-F5942ADBA4FC}"/>
   </bookViews>
   <sheets>
     <sheet name="ICP Level II N data" sheetId="1" r:id="rId1"/>
@@ -5609,8 +5609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFB1B43-A2CF-41A2-B653-1C573349BF1F}">
   <dimension ref="A1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F91" sqref="F66:F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8108,7 +8108,7 @@
         <v>32</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G66" s="10">
         <v>1994</v>
@@ -8146,7 +8146,7 @@
         <v>32</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G67" s="10">
         <v>1995</v>
@@ -8184,7 +8184,7 @@
         <v>32</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G68" s="10">
         <v>1996</v>
@@ -8222,7 +8222,7 @@
         <v>32</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G69" s="10">
         <v>1997</v>
@@ -8260,7 +8260,7 @@
         <v>32</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G70" s="10">
         <v>1998</v>
@@ -8298,7 +8298,7 @@
         <v>32</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G71" s="10">
         <v>1999</v>
@@ -8336,7 +8336,7 @@
         <v>32</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G72" s="10">
         <v>2000</v>
@@ -8374,7 +8374,7 @@
         <v>32</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G73" s="10">
         <v>2001</v>
@@ -8412,7 +8412,7 @@
         <v>32</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G74" s="10">
         <v>2002</v>
@@ -8450,7 +8450,7 @@
         <v>32</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G75" s="10">
         <v>2003</v>
@@ -8488,7 +8488,7 @@
         <v>32</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G76" s="10">
         <v>2004</v>
@@ -8526,7 +8526,7 @@
         <v>32</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G77" s="10">
         <v>2005</v>
@@ -8564,7 +8564,7 @@
         <v>32</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G78" s="10">
         <v>2006</v>
@@ -8602,7 +8602,7 @@
         <v>32</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G79" s="10">
         <v>2007</v>
@@ -8640,7 +8640,7 @@
         <v>32</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G80" s="10">
         <v>2008</v>
@@ -8678,7 +8678,7 @@
         <v>32</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G81" s="10">
         <v>2009</v>
@@ -8716,7 +8716,7 @@
         <v>32</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G82" s="10">
         <v>2010</v>
@@ -8754,7 +8754,7 @@
         <v>32</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G83" s="10">
         <v>2011</v>
@@ -8792,7 +8792,7 @@
         <v>32</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G84" s="10">
         <v>2012</v>
@@ -8830,7 +8830,7 @@
         <v>32</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G85" s="10">
         <v>2013</v>
@@ -8868,7 +8868,7 @@
         <v>32</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G86" s="10">
         <v>2014</v>
@@ -8906,7 +8906,7 @@
         <v>32</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G87" s="10">
         <v>2015</v>
@@ -8944,7 +8944,7 @@
         <v>32</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G88" s="10">
         <v>2016</v>
@@ -8982,7 +8982,7 @@
         <v>32</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G89" s="10">
         <v>2017</v>
@@ -9020,7 +9020,7 @@
         <v>32</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G90" s="10">
         <v>2018</v>
@@ -9058,7 +9058,7 @@
         <v>32</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G91" s="10">
         <v>2019</v>

</xml_diff>

<commit_message>
final analysis with updated data from Romania
</commit_message>
<xml_diff>
--- a/data/ICP_Level_II_sites_N_data_2021.xlsx
+++ b/data/ICP_Level_II_sites_N_data_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Tresch IAP\Desktop\IAP\1_Projects\11_UNECE\N_leaching_CLempN\N_leaching_analysis_CLempN\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68B48F6-5362-4669-94E0-A01BC6ED77BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B98E58-BCF4-4ECF-BD52-CE3DD167FC81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="2" xr2:uid="{4B878E5B-3B0D-4C3A-956A-F5942ADBA4FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4B878E5B-3B0D-4C3A-956A-F5942ADBA4FC}"/>
   </bookViews>
   <sheets>
     <sheet name="ICP Level II N data" sheetId="1" r:id="rId1"/>
@@ -768,7 +768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
+    <sheetView topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="H38" sqref="H34:H38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1826,6 +1828,9 @@
         <f>AVERAGE('annual data'!H118:H122)</f>
         <v>13.92342857142857</v>
       </c>
+      <c r="H34">
+        <v>25.082361913668905</v>
+      </c>
       <c r="I34" s="5" t="s">
         <v>97</v>
       </c>
@@ -1855,8 +1860,8 @@
         <f>AVERAGE('annual data'!H123:H127)</f>
         <v>32.363999999999997</v>
       </c>
-      <c r="H35" s="5">
-        <v>2.0499999999999998</v>
+      <c r="H35">
+        <v>24.43652618135377</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>97</v>
@@ -1884,8 +1889,8 @@
         <f>AVERAGE('annual data'!H128:H132)</f>
         <v>22.506</v>
       </c>
-      <c r="H36" s="5">
-        <v>2.0299999999999998</v>
+      <c r="H36">
+        <v>25.071010860484545</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>97</v>
@@ -1917,7 +1922,7 @@
         <v>15.326857142857145</v>
       </c>
       <c r="H37">
-        <v>1.71</v>
+        <v>19.732025406847821</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>97</v>
@@ -1948,8 +1953,8 @@
         <f>AVERAGE('annual data'!H138:H142)</f>
         <v>24.33942857142857</v>
       </c>
-      <c r="H38" s="5">
-        <v>2.79</v>
+      <c r="H38">
+        <v>27.158369068451201</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>97</v>
@@ -1969,8 +1974,8 @@
   <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A138" sqref="A138:C138"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F138" sqref="F138:H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5609,8 +5614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFB1B43-A2CF-41A2-B653-1C573349BF1F}">
   <dimension ref="A1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="F91" sqref="F66:F91"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="M142" sqref="M142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10824,7 +10829,9 @@
       <c r="J141">
         <v>13.92342857142857</v>
       </c>
-      <c r="L141" s="5"/>
+      <c r="L141" s="5">
+        <v>25.082361913668905</v>
+      </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
@@ -10852,7 +10859,7 @@
         <v>32.363999999999997</v>
       </c>
       <c r="L142" s="5">
-        <v>2.0499999999999998</v>
+        <v>24.43652618135377</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
@@ -10881,7 +10888,7 @@
         <v>22.506</v>
       </c>
       <c r="L143" s="5">
-        <v>2.0299999999999998</v>
+        <v>25.071010860484545</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
@@ -10910,7 +10917,7 @@
         <v>15.326857142857145</v>
       </c>
       <c r="L144" s="5">
-        <v>1.71</v>
+        <v>19.732025406847821</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
@@ -10939,7 +10946,7 @@
         <v>24.33942857142857</v>
       </c>
       <c r="L145" s="5">
-        <v>2.79</v>
+        <v>27.158369068451201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>